<commit_message>
add chart setDataRange() example
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/chart.xlsx
+++ b/src/main/webapp/WEB-INF/books/chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A49A6EC-C66A-FF48-9704-CA9FAAC0AB9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2A7C30-156C-AD46-A972-1302C0975B1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="20120" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="20120" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="chart" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Chrome</t>
   </si>
@@ -47,6 +47,30 @@
   </si>
   <si>
     <t>Browser market share 2013</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Banna</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Melon</t>
+  </si>
+  <si>
+    <t>Cherry</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>Pineapple</t>
   </si>
 </sst>
 </file>
@@ -312,6 +336,28 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2DD6448C-7157-494C-A37B-AA2FAE36F693}" name="Table2" displayName="Table2" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{C0998D67-BD14-9C4F-8E9D-00990B2A170C}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CEAB1B5B-AF5A-DF48-8750-ECC2D376D95F}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{2739183B-892E-C049-B5AF-702756CC1D2D}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3EA6F3F9-DB3F-8244-898B-F2DB32B8180C}" name="Table24" displayName="Table24" ref="A10:B16" totalsRowShown="0">
+  <autoFilter ref="A10:B16" xr:uid="{491CCC50-FFA9-514A-A0FF-7DB51EC43BCA}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{762642F2-EAC8-664C-B590-D658080F84B4}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{3D9CC222-6319-6C43-A1B0-E2FB6EC7CA57}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -635,67 +681,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B16" sqref="B11:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>44.6</v>
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>22.08</v>
+        <v>44.6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>18.170000000000002</v>
+        <v>22.08</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>9.07</v>
+        <v>18.170000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>3.38</v>
+        <v>9.07</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>3.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>